<commit_message>
Added Summary to Report
</commit_message>
<xml_diff>
--- a/Eval Metrics.xlsx
+++ b/Eval Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mental Health Illness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE1684-4300-4D88-9011-2CC75EB15D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A35532-82FE-4A29-AAA7-7B359C64DD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA67209A-CEB7-4E28-822D-377293D4975F}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N12" sqref="M12:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>